<commit_message>
generation d'images artifcielles réussi
</commit_message>
<xml_diff>
--- a/test_Projet_synthse.xlsx
+++ b/test_Projet_synthse.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/afsanehsheikhmiri/Documents/Afsaneh/Graduation_project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/afsanehsheikhmiri/Documents/Afsaneh/git_graduation_project/projet_synthese_HIV2020/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16440" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16400" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="graph" sheetId="2" r:id="rId1"/>
@@ -3118,12 +3118,12 @@
             </c:spPr>
           </c:bandFmt>
         </c:bandFmts>
-        <c:axId val="-439929744"/>
-        <c:axId val="-439972784"/>
-        <c:axId val="-439591920"/>
+        <c:axId val="-640786880"/>
+        <c:axId val="-640816320"/>
+        <c:axId val="-641449712"/>
       </c:surface3DChart>
       <c:catAx>
-        <c:axId val="-439929744"/>
+        <c:axId val="-640786880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3166,7 +3166,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-439972784"/>
+        <c:crossAx val="-640816320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3174,7 +3174,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-439972784"/>
+        <c:axId val="-640816320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3224,12 +3224,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-439929744"/>
+        <c:crossAx val="-640786880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="-439591920"/>
+        <c:axId val="-641449712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3271,7 +3271,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-439972784"/>
+        <c:crossAx val="-640816320"/>
         <c:crosses val="autoZero"/>
       </c:serAx>
       <c:spPr>
@@ -6548,12 +6548,12 @@
             </c:spPr>
           </c:bandFmt>
         </c:bandFmts>
-        <c:axId val="-356470912"/>
-        <c:axId val="-356468864"/>
-        <c:axId val="-356490240"/>
+        <c:axId val="-613777840"/>
+        <c:axId val="-613775776"/>
+        <c:axId val="-613773296"/>
       </c:surface3DChart>
       <c:catAx>
-        <c:axId val="-356470912"/>
+        <c:axId val="-613777840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6596,7 +6596,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-356468864"/>
+        <c:crossAx val="-613775776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6604,7 +6604,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-356468864"/>
+        <c:axId val="-613775776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6654,12 +6654,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-356470912"/>
+        <c:crossAx val="-613777840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="-356490240"/>
+        <c:axId val="-613773296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6701,7 +6701,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-356468864"/>
+        <c:crossAx val="-613775776"/>
         <c:crosses val="autoZero"/>
       </c:serAx>
       <c:spPr>
@@ -6714,6 +6714,98 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:legendEntry>
+        <c:idx val="0"/>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr rtl="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="1"/>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr rtl="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="2"/>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr rtl="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="3"/>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr rtl="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+      </c:legendEntry>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -6824,15 +6916,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>673100</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
+      <xdr:colOff>660400</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>292100</xdr:colOff>
+      <xdr:colOff>279400</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7121,7 +7213,7 @@
   <dimension ref="A2:T35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N34" sqref="N34"/>
+      <selection activeCell="P26" sqref="P26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8717,25 +8809,25 @@
         <v>0</v>
       </c>
       <c r="B28">
-        <v>7</v>
+        <v>233.33</v>
       </c>
       <c r="D28" t="s">
         <v>0</v>
       </c>
       <c r="E28">
-        <v>5</v>
+        <v>166.67</v>
       </c>
       <c r="G28" t="s">
         <v>0</v>
       </c>
       <c r="H28">
-        <v>9</v>
+        <v>300</v>
       </c>
       <c r="J28" t="s">
         <v>0</v>
       </c>
       <c r="K28">
-        <v>7</v>
+        <v>233.33</v>
       </c>
       <c r="M28" t="s">
         <v>0</v>
@@ -8749,25 +8841,25 @@
         <v>1</v>
       </c>
       <c r="B29">
-        <v>10</v>
+        <v>325</v>
       </c>
       <c r="D29" t="s">
         <v>1</v>
       </c>
       <c r="E29">
-        <v>13</v>
+        <v>325</v>
       </c>
       <c r="G29" t="s">
         <v>1</v>
       </c>
       <c r="H29">
-        <v>8</v>
+        <v>200</v>
       </c>
       <c r="J29" t="s">
         <v>1</v>
       </c>
       <c r="K29">
-        <v>13</v>
+        <v>325</v>
       </c>
       <c r="M29" t="s">
         <v>1</v>
@@ -8781,25 +8873,25 @@
         <v>2</v>
       </c>
       <c r="B30">
-        <v>5</v>
+        <v>166.67</v>
       </c>
       <c r="D30" t="s">
         <v>2</v>
       </c>
       <c r="E30">
-        <v>3</v>
+        <v>100</v>
       </c>
       <c r="G30" t="s">
         <v>2</v>
       </c>
       <c r="H30">
-        <v>4</v>
+        <v>133.33000000000001</v>
       </c>
       <c r="J30" t="s">
         <v>2</v>
       </c>
       <c r="K30">
-        <v>3</v>
+        <v>100</v>
       </c>
       <c r="M30" t="s">
         <v>2</v>
@@ -8813,25 +8905,25 @@
         <v>3</v>
       </c>
       <c r="B31">
-        <v>3</v>
+        <v>75</v>
       </c>
       <c r="D31" t="s">
         <v>3</v>
       </c>
       <c r="E31">
-        <v>2</v>
+        <v>50</v>
       </c>
       <c r="G31" t="s">
         <v>3</v>
       </c>
       <c r="H31">
-        <v>3</v>
+        <v>100</v>
       </c>
       <c r="J31" t="s">
         <v>3</v>
       </c>
       <c r="K31">
-        <v>2</v>
+        <v>50</v>
       </c>
       <c r="M31" t="s">
         <v>3</v>
@@ -8845,7 +8937,7 @@
         <v>4</v>
       </c>
       <c r="B32">
-        <v>55</v>
+        <v>100</v>
       </c>
       <c r="D32" t="s">
         <v>4</v>
@@ -8877,25 +8969,25 @@
         <v>5</v>
       </c>
       <c r="B33">
-        <v>2</v>
+        <v>40</v>
       </c>
       <c r="D33" t="s">
         <v>5</v>
       </c>
       <c r="E33">
-        <v>4</v>
+        <v>80</v>
       </c>
       <c r="G33" t="s">
         <v>5</v>
       </c>
       <c r="H33">
-        <v>5</v>
+        <v>60</v>
       </c>
       <c r="J33" t="s">
         <v>5</v>
       </c>
       <c r="K33">
-        <v>2</v>
+        <v>40</v>
       </c>
       <c r="M33" t="s">
         <v>5</v>

</xml_diff>